<commit_message>
curated datasets for different Al grades
</commit_message>
<xml_diff>
--- a/data/averaged_filtered_AA1000.xlsx
+++ b/data/averaged_filtered_AA1000.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F309"/>
+  <dimension ref="A1:F334"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5924,815 +5924,815 @@
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>NC1=CCNC(=S)N1</t>
+          <t>NC(N)=S</t>
         </is>
       </c>
       <c r="B250" t="n">
-        <v>1</v>
+        <v>144</v>
       </c>
       <c r="C250" t="n">
-        <v>0</v>
+        <v>-0.1367205671564068</v>
       </c>
       <c r="D250" t="n">
-        <v>1e-07</v>
+        <v>0.66</v>
       </c>
       <c r="E250" t="n">
         <v>0</v>
       </c>
       <c r="F250" t="n">
-        <v>66.06</v>
+        <v>28.59</v>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>NC1=CCNC(=S)N1</t>
+          <t>NC(N)=S</t>
         </is>
       </c>
       <c r="B251" t="n">
-        <v>1</v>
+        <v>144</v>
       </c>
       <c r="C251" t="n">
-        <v>0</v>
+        <v>-0.1367205671564068</v>
       </c>
       <c r="D251" t="n">
-        <v>1e-06</v>
+        <v>1.32</v>
       </c>
       <c r="E251" t="n">
         <v>0</v>
       </c>
       <c r="F251" t="n">
-        <v>77.15000000000001</v>
+        <v>35.28</v>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>NC1=CCNC(=S)N1</t>
+          <t>NC(N)=S</t>
         </is>
       </c>
       <c r="B252" t="n">
-        <v>1</v>
+        <v>144</v>
       </c>
       <c r="C252" t="n">
-        <v>0</v>
+        <v>-0.1367205671564068</v>
       </c>
       <c r="D252" t="n">
-        <v>1e-05</v>
+        <v>1.97</v>
       </c>
       <c r="E252" t="n">
         <v>0</v>
       </c>
       <c r="F252" t="n">
-        <v>85.84</v>
+        <v>36.85</v>
       </c>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>NC1=CCNC(=S)N1</t>
+          <t>NC(N)=S</t>
         </is>
       </c>
       <c r="B253" t="n">
-        <v>1</v>
+        <v>144</v>
       </c>
       <c r="C253" t="n">
-        <v>0</v>
+        <v>-0.1367205671564068</v>
       </c>
       <c r="D253" t="n">
-        <v>0.0001</v>
+        <v>2.63</v>
       </c>
       <c r="E253" t="n">
         <v>0</v>
       </c>
       <c r="F253" t="n">
-        <v>91.06</v>
+        <v>39.59</v>
       </c>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>NC1=CCNC(=S)N1</t>
+          <t>NC(N)=S</t>
         </is>
       </c>
       <c r="B254" t="n">
-        <v>1</v>
+        <v>144</v>
       </c>
       <c r="C254" t="n">
-        <v>0</v>
+        <v>-0.1367205671564068</v>
       </c>
       <c r="D254" t="n">
-        <v>0.001</v>
+        <v>3.28</v>
       </c>
       <c r="E254" t="n">
         <v>0</v>
       </c>
       <c r="F254" t="n">
-        <v>90.66333333333334</v>
+        <v>40.31</v>
       </c>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>OC1=C(C=CC=C1)C=NC2=CC=C(C=C2)N=NC3=C(C=CC=C3)N=CC4=C(C=CC=C4)O</t>
+          <t>NC(N)=S</t>
         </is>
       </c>
       <c r="B255" t="n">
-        <v>1</v>
+        <v>288</v>
       </c>
       <c r="C255" t="n">
-        <v>13</v>
+        <v>-0.1367205671564068</v>
       </c>
       <c r="D255" t="n">
-        <v>0.001</v>
+        <v>0.66</v>
       </c>
       <c r="E255" t="n">
         <v>0</v>
       </c>
       <c r="F255" t="n">
-        <v>29.7</v>
+        <v>30.87</v>
       </c>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>OC1=C(C=CC=C1)C=NC2=CC=C(C=C2)N=NC3=C(C=CC=C3)N=CC4=C(C=CC=C4)O</t>
+          <t>NC(N)=S</t>
         </is>
       </c>
       <c r="B256" t="n">
-        <v>1</v>
+        <v>288</v>
       </c>
       <c r="C256" t="n">
-        <v>13</v>
+        <v>-0.1367205671564068</v>
       </c>
       <c r="D256" t="n">
-        <v>0.005</v>
+        <v>1.32</v>
       </c>
       <c r="E256" t="n">
         <v>0</v>
       </c>
       <c r="F256" t="n">
-        <v>40.03333333333333</v>
+        <v>37.1</v>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>OC1=C(C=CC=C1)C=NC2=CC=C(C=C2)N=NC3=C(C=CC=C3)N=CC4=C(C=CC=C4)O</t>
+          <t>NC(N)=S</t>
         </is>
       </c>
       <c r="B257" t="n">
-        <v>1</v>
+        <v>288</v>
       </c>
       <c r="C257" t="n">
-        <v>13</v>
+        <v>-0.1367205671564068</v>
       </c>
       <c r="D257" t="n">
-        <v>0.01</v>
+        <v>1.97</v>
       </c>
       <c r="E257" t="n">
         <v>0</v>
       </c>
       <c r="F257" t="n">
-        <v>47.06666666666666</v>
+        <v>40.09</v>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>OC1=CN=N[N]1C2=CC=C(C=C2)Cl</t>
+          <t>NC(N)=S</t>
         </is>
       </c>
       <c r="B258" t="n">
-        <v>0.5</v>
+        <v>288</v>
       </c>
       <c r="C258" t="n">
-        <v>0</v>
+        <v>-0.1367205671564068</v>
       </c>
       <c r="D258" t="n">
-        <v>0.0003</v>
+        <v>2.63</v>
       </c>
       <c r="E258" t="n">
         <v>0</v>
       </c>
       <c r="F258" t="n">
-        <v>20.036</v>
+        <v>39.06</v>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>OC1=CN=N[N]1C2=CC=C(C=C2)Cl</t>
+          <t>NC(N)=S</t>
         </is>
       </c>
       <c r="B259" t="n">
-        <v>0.5</v>
+        <v>288</v>
       </c>
       <c r="C259" t="n">
-        <v>0</v>
+        <v>-0.1367205671564068</v>
       </c>
       <c r="D259" t="n">
-        <v>0.0005</v>
+        <v>3.28</v>
       </c>
       <c r="E259" t="n">
         <v>0</v>
       </c>
       <c r="F259" t="n">
-        <v>28.34</v>
+        <v>42.02</v>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>OC1=CN=N[N]1C2=CC=C(C=C2)Cl</t>
+          <t>NC(N)=S</t>
         </is>
       </c>
       <c r="B260" t="n">
-        <v>0.5</v>
+        <v>432</v>
       </c>
       <c r="C260" t="n">
-        <v>0</v>
+        <v>-0.1367205671564068</v>
       </c>
       <c r="D260" t="n">
-        <v>0.001</v>
+        <v>0.66</v>
       </c>
       <c r="E260" t="n">
         <v>0</v>
       </c>
       <c r="F260" t="n">
-        <v>38.944</v>
+        <v>31.55</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>OC1=CN=N[N]1C2=CC=C(C=C2)Cl</t>
+          <t>NC(N)=S</t>
         </is>
       </c>
       <c r="B261" t="n">
-        <v>0.5</v>
+        <v>432</v>
       </c>
       <c r="C261" t="n">
-        <v>0</v>
+        <v>-0.1367205671564068</v>
       </c>
       <c r="D261" t="n">
-        <v>0.003</v>
+        <v>1.32</v>
       </c>
       <c r="E261" t="n">
         <v>0</v>
       </c>
       <c r="F261" t="n">
-        <v>50.22799999999999</v>
+        <v>37.5</v>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>S=c1sc2c([nH]1)cccc2</t>
+          <t>NC(N)=S</t>
         </is>
       </c>
       <c r="B262" t="n">
-        <v>48</v>
+        <v>432</v>
       </c>
       <c r="C262" t="n">
-        <v>-0.6</v>
+        <v>-0.1367205671564068</v>
       </c>
       <c r="D262" t="n">
-        <v>0.0032</v>
+        <v>1.97</v>
       </c>
       <c r="E262" t="n">
         <v>0</v>
       </c>
       <c r="F262" t="n">
-        <v>41.35</v>
+        <v>40.86</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>S=c1sc2c([nH]1)cccc2</t>
+          <t>NC(N)=S</t>
         </is>
       </c>
       <c r="B263" t="n">
-        <v>48</v>
+        <v>432</v>
       </c>
       <c r="C263" t="n">
-        <v>-0.6</v>
+        <v>-0.1367205671564068</v>
       </c>
       <c r="D263" t="n">
-        <v>0.0042</v>
+        <v>2.63</v>
       </c>
       <c r="E263" t="n">
         <v>0</v>
       </c>
       <c r="F263" t="n">
-        <v>19.74</v>
+        <v>41.28</v>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>S=c1sc2c([nH]1)cccc2</t>
+          <t>NC(N)=S</t>
         </is>
       </c>
       <c r="B264" t="n">
-        <v>48</v>
+        <v>432</v>
       </c>
       <c r="C264" t="n">
-        <v>-0.6</v>
+        <v>-0.1367205671564068</v>
       </c>
       <c r="D264" t="n">
-        <v>0.0053</v>
+        <v>3.28</v>
       </c>
       <c r="E264" t="n">
         <v>0</v>
       </c>
       <c r="F264" t="n">
-        <v>18.8</v>
+        <v>45.32</v>
       </c>
     </row>
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>S=c1sc2c([nH]1)cccc2</t>
+          <t>NC(N)=S</t>
         </is>
       </c>
       <c r="B265" t="n">
-        <v>48</v>
+        <v>576</v>
       </c>
       <c r="C265" t="n">
-        <v>-0.6</v>
+        <v>-0.1367205671564068</v>
       </c>
       <c r="D265" t="n">
-        <v>0.0065</v>
+        <v>0.66</v>
       </c>
       <c r="E265" t="n">
         <v>0</v>
       </c>
       <c r="F265" t="n">
-        <v>15.79</v>
+        <v>35.57</v>
       </c>
     </row>
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>S=c1sc2c([nH]1)cccc2</t>
+          <t>NC(N)=S</t>
         </is>
       </c>
       <c r="B266" t="n">
-        <v>48</v>
+        <v>576</v>
       </c>
       <c r="C266" t="n">
-        <v>-0.6</v>
+        <v>-0.1367205671564068</v>
       </c>
       <c r="D266" t="n">
-        <v>0.0075</v>
+        <v>1.32</v>
       </c>
       <c r="E266" t="n">
         <v>0</v>
       </c>
       <c r="F266" t="n">
-        <v>-0.5600000000000001</v>
+        <v>37.32</v>
       </c>
     </row>
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>S=c1sc2c([nH]1)cccc2</t>
+          <t>NC(N)=S</t>
         </is>
       </c>
       <c r="B267" t="n">
-        <v>48</v>
+        <v>576</v>
       </c>
       <c r="C267" t="n">
-        <v>-0.6</v>
+        <v>-0.1367205671564068</v>
       </c>
       <c r="D267" t="n">
-        <v>0.008500000000000001</v>
+        <v>1.97</v>
       </c>
       <c r="E267" t="n">
         <v>0</v>
       </c>
       <c r="F267" t="n">
-        <v>21.05</v>
+        <v>43.9</v>
       </c>
     </row>
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>S=c1sc2c([nH]1)cccc2</t>
+          <t>NC(N)=S</t>
         </is>
       </c>
       <c r="B268" t="n">
-        <v>96</v>
+        <v>576</v>
       </c>
       <c r="C268" t="n">
-        <v>-0.6</v>
+        <v>-0.1367205671564068</v>
       </c>
       <c r="D268" t="n">
-        <v>0.0032</v>
+        <v>2.63</v>
       </c>
       <c r="E268" t="n">
         <v>0</v>
       </c>
       <c r="F268" t="n">
-        <v>42.57</v>
+        <v>47.54</v>
       </c>
     </row>
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>S=c1sc2c([nH]1)cccc2</t>
+          <t>NC(N)=S</t>
         </is>
       </c>
       <c r="B269" t="n">
-        <v>96</v>
+        <v>576</v>
       </c>
       <c r="C269" t="n">
-        <v>-0.6</v>
+        <v>-0.1367205671564068</v>
       </c>
       <c r="D269" t="n">
-        <v>0.0042</v>
+        <v>3.28</v>
       </c>
       <c r="E269" t="n">
         <v>0</v>
       </c>
       <c r="F269" t="n">
-        <v>-33.11</v>
+        <v>51.31</v>
       </c>
     </row>
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>S=c1sc2c([nH]1)cccc2</t>
+          <t>NC(N)=S</t>
         </is>
       </c>
       <c r="B270" t="n">
-        <v>96</v>
+        <v>720</v>
       </c>
       <c r="C270" t="n">
-        <v>-0.6</v>
+        <v>-0.1367205671564068</v>
       </c>
       <c r="D270" t="n">
-        <v>0.0053</v>
+        <v>0.66</v>
       </c>
       <c r="E270" t="n">
         <v>0</v>
       </c>
       <c r="F270" t="n">
-        <v>6.22</v>
+        <v>39.33</v>
       </c>
     </row>
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>S=c1sc2c([nH]1)cccc2</t>
+          <t>NC(N)=S</t>
         </is>
       </c>
       <c r="B271" t="n">
-        <v>96</v>
+        <v>720</v>
       </c>
       <c r="C271" t="n">
-        <v>-0.6</v>
+        <v>-0.1367205671564068</v>
       </c>
       <c r="D271" t="n">
-        <v>0.0065</v>
+        <v>1.32</v>
       </c>
       <c r="E271" t="n">
         <v>0</v>
       </c>
       <c r="F271" t="n">
-        <v>17.57</v>
+        <v>46.85</v>
       </c>
     </row>
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>S=c1sc2c([nH]1)cccc2</t>
+          <t>NC(N)=S</t>
         </is>
       </c>
       <c r="B272" t="n">
-        <v>96</v>
+        <v>720</v>
       </c>
       <c r="C272" t="n">
-        <v>-0.6</v>
+        <v>-0.1367205671564068</v>
       </c>
       <c r="D272" t="n">
-        <v>0.0075</v>
+        <v>1.97</v>
       </c>
       <c r="E272" t="n">
         <v>0</v>
       </c>
       <c r="F272" t="n">
-        <v>18.24</v>
+        <v>47.4</v>
       </c>
     </row>
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>S=c1sc2c([nH]1)cccc2</t>
+          <t>NC(N)=S</t>
         </is>
       </c>
       <c r="B273" t="n">
-        <v>96</v>
+        <v>720</v>
       </c>
       <c r="C273" t="n">
-        <v>-0.6</v>
+        <v>-0.1367205671564068</v>
       </c>
       <c r="D273" t="n">
-        <v>0.008500000000000001</v>
+        <v>2.63</v>
       </c>
       <c r="E273" t="n">
         <v>0</v>
       </c>
       <c r="F273" t="n">
-        <v>22.97</v>
+        <v>49.87</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>S=c1sc2c([nH]1)cccc2</t>
+          <t>NC(N)=S</t>
         </is>
       </c>
       <c r="B274" t="n">
-        <v>144</v>
+        <v>720</v>
       </c>
       <c r="C274" t="n">
-        <v>-0.6</v>
+        <v>-0.1367205671564068</v>
       </c>
       <c r="D274" t="n">
-        <v>0.0032</v>
+        <v>3.28</v>
       </c>
       <c r="E274" t="n">
         <v>0</v>
       </c>
       <c r="F274" t="n">
-        <v>12.71</v>
+        <v>52.54</v>
       </c>
     </row>
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>S=c1sc2c([nH]1)cccc2</t>
+          <t>NC1=CCNC(=S)N1</t>
         </is>
       </c>
       <c r="B275" t="n">
-        <v>144</v>
+        <v>1</v>
       </c>
       <c r="C275" t="n">
-        <v>-0.6</v>
+        <v>0</v>
       </c>
       <c r="D275" t="n">
-        <v>0.0042</v>
+        <v>1e-07</v>
       </c>
       <c r="E275" t="n">
         <v>0</v>
       </c>
       <c r="F275" t="n">
-        <v>-49.17</v>
+        <v>66.06</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>S=c1sc2c([nH]1)cccc2</t>
+          <t>NC1=CCNC(=S)N1</t>
         </is>
       </c>
       <c r="B276" t="n">
-        <v>144</v>
+        <v>1</v>
       </c>
       <c r="C276" t="n">
-        <v>-0.6</v>
+        <v>0</v>
       </c>
       <c r="D276" t="n">
-        <v>0.0053</v>
+        <v>1e-06</v>
       </c>
       <c r="E276" t="n">
         <v>0</v>
       </c>
       <c r="F276" t="n">
-        <v>6.08</v>
+        <v>77.15000000000001</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>S=c1sc2c([nH]1)cccc2</t>
+          <t>NC1=CCNC(=S)N1</t>
         </is>
       </c>
       <c r="B277" t="n">
-        <v>144</v>
+        <v>1</v>
       </c>
       <c r="C277" t="n">
-        <v>-0.6</v>
+        <v>0</v>
       </c>
       <c r="D277" t="n">
-        <v>0.0065</v>
+        <v>1e-05</v>
       </c>
       <c r="E277" t="n">
         <v>0</v>
       </c>
       <c r="F277" t="n">
-        <v>19.34</v>
+        <v>85.84</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>S=c1sc2c([nH]1)cccc2</t>
+          <t>NC1=CCNC(=S)N1</t>
         </is>
       </c>
       <c r="B278" t="n">
-        <v>144</v>
+        <v>1</v>
       </c>
       <c r="C278" t="n">
-        <v>-0.6</v>
+        <v>0</v>
       </c>
       <c r="D278" t="n">
-        <v>0.0075</v>
+        <v>0.0001</v>
       </c>
       <c r="E278" t="n">
         <v>0</v>
       </c>
       <c r="F278" t="n">
-        <v>13.26</v>
+        <v>91.06</v>
       </c>
     </row>
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>S=c1sc2c([nH]1)cccc2</t>
+          <t>NC1=CCNC(=S)N1</t>
         </is>
       </c>
       <c r="B279" t="n">
-        <v>144</v>
+        <v>1</v>
       </c>
       <c r="C279" t="n">
-        <v>-0.6</v>
+        <v>0</v>
       </c>
       <c r="D279" t="n">
-        <v>0.008500000000000001</v>
+        <v>0.001</v>
       </c>
       <c r="E279" t="n">
         <v>0</v>
       </c>
       <c r="F279" t="n">
-        <v>22.76</v>
+        <v>90.66333333333334</v>
       </c>
     </row>
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>S=c1sc2c([nH]1)cccc2</t>
+          <t>OC1=C(C=CC=C1)C=NC2=CC=C(C=C2)N=NC3=C(C=CC=C3)N=CC4=C(C=CC=C4)O</t>
         </is>
       </c>
       <c r="B280" t="n">
-        <v>192</v>
+        <v>1</v>
       </c>
       <c r="C280" t="n">
-        <v>-0.6</v>
+        <v>13</v>
       </c>
       <c r="D280" t="n">
-        <v>0.0032</v>
+        <v>0.001</v>
       </c>
       <c r="E280" t="n">
         <v>0</v>
       </c>
       <c r="F280" t="n">
-        <v>56.85</v>
+        <v>29.7</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>S=c1sc2c([nH]1)cccc2</t>
+          <t>OC1=C(C=CC=C1)C=NC2=CC=C(C=C2)N=NC3=C(C=CC=C3)N=CC4=C(C=CC=C4)O</t>
         </is>
       </c>
       <c r="B281" t="n">
-        <v>192</v>
+        <v>1</v>
       </c>
       <c r="C281" t="n">
-        <v>-0.6</v>
+        <v>13</v>
       </c>
       <c r="D281" t="n">
-        <v>0.0042</v>
+        <v>0.005</v>
       </c>
       <c r="E281" t="n">
         <v>0</v>
       </c>
       <c r="F281" t="n">
-        <v>31.54</v>
+        <v>40.03333333333333</v>
       </c>
     </row>
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>S=c1sc2c([nH]1)cccc2</t>
+          <t>OC1=C(C=CC=C1)C=NC2=CC=C(C=C2)N=NC3=C(C=CC=C3)N=CC4=C(C=CC=C4)O</t>
         </is>
       </c>
       <c r="B282" t="n">
-        <v>192</v>
+        <v>1</v>
       </c>
       <c r="C282" t="n">
-        <v>-0.6</v>
+        <v>13</v>
       </c>
       <c r="D282" t="n">
-        <v>0.0053</v>
+        <v>0.01</v>
       </c>
       <c r="E282" t="n">
         <v>0</v>
       </c>
       <c r="F282" t="n">
-        <v>53.91</v>
+        <v>47.06666666666666</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>S=c1sc2c([nH]1)cccc2</t>
+          <t>OC1=CN=N[N]1C2=CC=C(C=C2)Cl</t>
         </is>
       </c>
       <c r="B283" t="n">
-        <v>192</v>
+        <v>0.5</v>
       </c>
       <c r="C283" t="n">
-        <v>-0.6</v>
+        <v>0</v>
       </c>
       <c r="D283" t="n">
-        <v>0.0065</v>
+        <v>0.0003</v>
       </c>
       <c r="E283" t="n">
         <v>0</v>
       </c>
       <c r="F283" t="n">
-        <v>60.69</v>
+        <v>20.036</v>
       </c>
     </row>
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>S=c1sc2c([nH]1)cccc2</t>
+          <t>OC1=CN=N[N]1C2=CC=C(C=C2)Cl</t>
         </is>
       </c>
       <c r="B284" t="n">
-        <v>192</v>
+        <v>0.5</v>
       </c>
       <c r="C284" t="n">
-        <v>-0.6</v>
+        <v>0</v>
       </c>
       <c r="D284" t="n">
-        <v>0.0075</v>
+        <v>0.0005</v>
       </c>
       <c r="E284" t="n">
         <v>0</v>
       </c>
       <c r="F284" t="n">
-        <v>55.94</v>
+        <v>28.34</v>
       </c>
     </row>
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>S=c1sc2c([nH]1)cccc2</t>
+          <t>OC1=CN=N[N]1C2=CC=C(C=C2)Cl</t>
         </is>
       </c>
       <c r="B285" t="n">
-        <v>192</v>
+        <v>0.5</v>
       </c>
       <c r="C285" t="n">
-        <v>-0.6</v>
+        <v>0</v>
       </c>
       <c r="D285" t="n">
-        <v>0.008500000000000001</v>
+        <v>0.001</v>
       </c>
       <c r="E285" t="n">
         <v>0</v>
       </c>
       <c r="F285" t="n">
-        <v>61.64</v>
+        <v>38.944</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>S=c1sc2c([nH]1)cccc2</t>
+          <t>OC1=CN=N[N]1C2=CC=C(C=C2)Cl</t>
         </is>
       </c>
       <c r="B286" t="n">
-        <v>240</v>
+        <v>0.5</v>
       </c>
       <c r="C286" t="n">
-        <v>-0.6</v>
+        <v>0</v>
       </c>
       <c r="D286" t="n">
-        <v>0.0032</v>
+        <v>0.003</v>
       </c>
       <c r="E286" t="n">
         <v>0</v>
       </c>
       <c r="F286" t="n">
-        <v>67.02</v>
+        <v>50.22799999999999</v>
       </c>
     </row>
     <row r="287">
@@ -6742,19 +6742,19 @@
         </is>
       </c>
       <c r="B287" t="n">
-        <v>240</v>
+        <v>48</v>
       </c>
       <c r="C287" t="n">
         <v>-0.6</v>
       </c>
       <c r="D287" t="n">
-        <v>0.0042</v>
+        <v>0.0032</v>
       </c>
       <c r="E287" t="n">
         <v>0</v>
       </c>
       <c r="F287" t="n">
-        <v>51.13</v>
+        <v>41.35</v>
       </c>
     </row>
     <row r="288">
@@ -6764,19 +6764,19 @@
         </is>
       </c>
       <c r="B288" t="n">
-        <v>240</v>
+        <v>48</v>
       </c>
       <c r="C288" t="n">
         <v>-0.6</v>
       </c>
       <c r="D288" t="n">
-        <v>0.0053</v>
+        <v>0.0042</v>
       </c>
       <c r="E288" t="n">
         <v>0</v>
       </c>
       <c r="F288" t="n">
-        <v>66.68000000000001</v>
+        <v>19.74</v>
       </c>
     </row>
     <row r="289">
@@ -6786,19 +6786,19 @@
         </is>
       </c>
       <c r="B289" t="n">
-        <v>240</v>
+        <v>48</v>
       </c>
       <c r="C289" t="n">
         <v>-0.6</v>
       </c>
       <c r="D289" t="n">
-        <v>0.0065</v>
+        <v>0.0053</v>
       </c>
       <c r="E289" t="n">
         <v>0</v>
       </c>
       <c r="F289" t="n">
-        <v>67.58</v>
+        <v>18.8</v>
       </c>
     </row>
     <row r="290">
@@ -6808,19 +6808,19 @@
         </is>
       </c>
       <c r="B290" t="n">
-        <v>240</v>
+        <v>48</v>
       </c>
       <c r="C290" t="n">
         <v>-0.6</v>
       </c>
       <c r="D290" t="n">
-        <v>0.0075</v>
+        <v>0.0065</v>
       </c>
       <c r="E290" t="n">
         <v>0</v>
       </c>
       <c r="F290" t="n">
-        <v>66.34</v>
+        <v>15.79</v>
       </c>
     </row>
     <row r="291">
@@ -6830,19 +6830,19 @@
         </is>
       </c>
       <c r="B291" t="n">
-        <v>240</v>
+        <v>48</v>
       </c>
       <c r="C291" t="n">
         <v>-0.6</v>
       </c>
       <c r="D291" t="n">
-        <v>0.008500000000000001</v>
+        <v>0.0075</v>
       </c>
       <c r="E291" t="n">
         <v>0</v>
       </c>
       <c r="F291" t="n">
-        <v>68.66</v>
+        <v>-0.5600000000000001</v>
       </c>
     </row>
     <row r="292">
@@ -6852,19 +6852,19 @@
         </is>
       </c>
       <c r="B292" t="n">
-        <v>288</v>
+        <v>48</v>
       </c>
       <c r="C292" t="n">
         <v>-0.6</v>
       </c>
       <c r="D292" t="n">
-        <v>0.0032</v>
+        <v>0.008500000000000001</v>
       </c>
       <c r="E292" t="n">
         <v>0</v>
       </c>
       <c r="F292" t="n">
-        <v>73.98999999999999</v>
+        <v>21.05</v>
       </c>
     </row>
     <row r="293">
@@ -6874,19 +6874,19 @@
         </is>
       </c>
       <c r="B293" t="n">
-        <v>288</v>
+        <v>96</v>
       </c>
       <c r="C293" t="n">
         <v>-0.6</v>
       </c>
       <c r="D293" t="n">
-        <v>0.0042</v>
+        <v>0.0032</v>
       </c>
       <c r="E293" t="n">
         <v>0</v>
       </c>
       <c r="F293" t="n">
-        <v>62.52</v>
+        <v>42.57</v>
       </c>
     </row>
     <row r="294">
@@ -6896,19 +6896,19 @@
         </is>
       </c>
       <c r="B294" t="n">
-        <v>288</v>
+        <v>96</v>
       </c>
       <c r="C294" t="n">
         <v>-0.6</v>
       </c>
       <c r="D294" t="n">
-        <v>0.0053</v>
+        <v>0.0042</v>
       </c>
       <c r="E294" t="n">
         <v>0</v>
       </c>
       <c r="F294" t="n">
-        <v>73.56</v>
+        <v>-33.11</v>
       </c>
     </row>
     <row r="295">
@@ -6918,19 +6918,19 @@
         </is>
       </c>
       <c r="B295" t="n">
-        <v>288</v>
+        <v>96</v>
       </c>
       <c r="C295" t="n">
         <v>-0.6</v>
       </c>
       <c r="D295" t="n">
-        <v>0.0065</v>
+        <v>0.0053</v>
       </c>
       <c r="E295" t="n">
         <v>0</v>
       </c>
       <c r="F295" t="n">
-        <v>72.56</v>
+        <v>6.22</v>
       </c>
     </row>
     <row r="296">
@@ -6940,19 +6940,19 @@
         </is>
       </c>
       <c r="B296" t="n">
-        <v>288</v>
+        <v>96</v>
       </c>
       <c r="C296" t="n">
         <v>-0.6</v>
       </c>
       <c r="D296" t="n">
-        <v>0.0075</v>
+        <v>0.0065</v>
       </c>
       <c r="E296" t="n">
         <v>0</v>
       </c>
       <c r="F296" t="n">
-        <v>71.72</v>
+        <v>17.57</v>
       </c>
     </row>
     <row r="297">
@@ -6962,19 +6962,19 @@
         </is>
       </c>
       <c r="B297" t="n">
-        <v>288</v>
+        <v>96</v>
       </c>
       <c r="C297" t="n">
         <v>-0.6</v>
       </c>
       <c r="D297" t="n">
-        <v>0.008500000000000001</v>
+        <v>0.0075</v>
       </c>
       <c r="E297" t="n">
         <v>0</v>
       </c>
       <c r="F297" t="n">
-        <v>73.38</v>
+        <v>18.24</v>
       </c>
     </row>
     <row r="298">
@@ -6984,19 +6984,19 @@
         </is>
       </c>
       <c r="B298" t="n">
-        <v>336</v>
+        <v>96</v>
       </c>
       <c r="C298" t="n">
         <v>-0.6</v>
       </c>
       <c r="D298" t="n">
-        <v>0.0032</v>
+        <v>0.008500000000000001</v>
       </c>
       <c r="E298" t="n">
         <v>0</v>
       </c>
       <c r="F298" t="n">
-        <v>76.83</v>
+        <v>22.97</v>
       </c>
     </row>
     <row r="299">
@@ -7006,19 +7006,19 @@
         </is>
       </c>
       <c r="B299" t="n">
-        <v>336</v>
+        <v>144</v>
       </c>
       <c r="C299" t="n">
         <v>-0.6</v>
       </c>
       <c r="D299" t="n">
-        <v>0.0042</v>
+        <v>0.0032</v>
       </c>
       <c r="E299" t="n">
         <v>0</v>
       </c>
       <c r="F299" t="n">
-        <v>69.75</v>
+        <v>12.71</v>
       </c>
     </row>
     <row r="300">
@@ -7028,19 +7028,19 @@
         </is>
       </c>
       <c r="B300" t="n">
-        <v>336</v>
+        <v>144</v>
       </c>
       <c r="C300" t="n">
         <v>-0.6</v>
       </c>
       <c r="D300" t="n">
-        <v>0.0053</v>
+        <v>0.0042</v>
       </c>
       <c r="E300" t="n">
         <v>0</v>
       </c>
       <c r="F300" t="n">
-        <v>78.36</v>
+        <v>-49.17</v>
       </c>
     </row>
     <row r="301">
@@ -7050,19 +7050,19 @@
         </is>
       </c>
       <c r="B301" t="n">
-        <v>336</v>
+        <v>144</v>
       </c>
       <c r="C301" t="n">
         <v>-0.6</v>
       </c>
       <c r="D301" t="n">
-        <v>0.0065</v>
+        <v>0.0053</v>
       </c>
       <c r="E301" t="n">
         <v>0</v>
       </c>
       <c r="F301" t="n">
-        <v>75.54000000000001</v>
+        <v>6.08</v>
       </c>
     </row>
     <row r="302">
@@ -7072,19 +7072,19 @@
         </is>
       </c>
       <c r="B302" t="n">
-        <v>336</v>
+        <v>144</v>
       </c>
       <c r="C302" t="n">
         <v>-0.6</v>
       </c>
       <c r="D302" t="n">
-        <v>0.0075</v>
+        <v>0.0065</v>
       </c>
       <c r="E302" t="n">
         <v>0</v>
       </c>
       <c r="F302" t="n">
-        <v>74.90000000000001</v>
+        <v>19.34</v>
       </c>
     </row>
     <row r="303">
@@ -7094,19 +7094,19 @@
         </is>
       </c>
       <c r="B303" t="n">
-        <v>336</v>
+        <v>144</v>
       </c>
       <c r="C303" t="n">
         <v>-0.6</v>
       </c>
       <c r="D303" t="n">
-        <v>0.008500000000000001</v>
+        <v>0.0075</v>
       </c>
       <c r="E303" t="n">
         <v>0</v>
       </c>
       <c r="F303" t="n">
-        <v>76.88</v>
+        <v>13.26</v>
       </c>
     </row>
     <row r="304">
@@ -7116,19 +7116,19 @@
         </is>
       </c>
       <c r="B304" t="n">
-        <v>384</v>
+        <v>144</v>
       </c>
       <c r="C304" t="n">
         <v>-0.6</v>
       </c>
       <c r="D304" t="n">
-        <v>0.0032</v>
+        <v>0.008500000000000001</v>
       </c>
       <c r="E304" t="n">
         <v>0</v>
       </c>
       <c r="F304" t="n">
-        <v>77.29000000000001</v>
+        <v>22.76</v>
       </c>
     </row>
     <row r="305">
@@ -7138,19 +7138,19 @@
         </is>
       </c>
       <c r="B305" t="n">
-        <v>384</v>
+        <v>192</v>
       </c>
       <c r="C305" t="n">
         <v>-0.6</v>
       </c>
       <c r="D305" t="n">
-        <v>0.0042</v>
+        <v>0.0032</v>
       </c>
       <c r="E305" t="n">
         <v>0</v>
       </c>
       <c r="F305" t="n">
-        <v>70.59999999999999</v>
+        <v>56.85</v>
       </c>
     </row>
     <row r="306">
@@ -7160,19 +7160,19 @@
         </is>
       </c>
       <c r="B306" t="n">
-        <v>384</v>
+        <v>192</v>
       </c>
       <c r="C306" t="n">
         <v>-0.6</v>
       </c>
       <c r="D306" t="n">
-        <v>0.0053</v>
+        <v>0.0042</v>
       </c>
       <c r="E306" t="n">
         <v>0</v>
       </c>
       <c r="F306" t="n">
-        <v>79.77</v>
+        <v>31.54</v>
       </c>
     </row>
     <row r="307">
@@ -7182,19 +7182,19 @@
         </is>
       </c>
       <c r="B307" t="n">
-        <v>384</v>
+        <v>192</v>
       </c>
       <c r="C307" t="n">
         <v>-0.6</v>
       </c>
       <c r="D307" t="n">
-        <v>0.0065</v>
+        <v>0.0053</v>
       </c>
       <c r="E307" t="n">
         <v>0</v>
       </c>
       <c r="F307" t="n">
-        <v>76.72</v>
+        <v>53.91</v>
       </c>
     </row>
     <row r="308">
@@ -7204,19 +7204,19 @@
         </is>
       </c>
       <c r="B308" t="n">
-        <v>384</v>
+        <v>192</v>
       </c>
       <c r="C308" t="n">
         <v>-0.6</v>
       </c>
       <c r="D308" t="n">
-        <v>0.0075</v>
+        <v>0.0065</v>
       </c>
       <c r="E308" t="n">
         <v>0</v>
       </c>
       <c r="F308" t="n">
-        <v>75.44</v>
+        <v>60.69</v>
       </c>
     </row>
     <row r="309">
@@ -7226,18 +7226,568 @@
         </is>
       </c>
       <c r="B309" t="n">
-        <v>384</v>
+        <v>192</v>
       </c>
       <c r="C309" t="n">
         <v>-0.6</v>
       </c>
       <c r="D309" t="n">
+        <v>0.0075</v>
+      </c>
+      <c r="E309" t="n">
+        <v>0</v>
+      </c>
+      <c r="F309" t="n">
+        <v>55.94</v>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>S=c1sc2c([nH]1)cccc2</t>
+        </is>
+      </c>
+      <c r="B310" t="n">
+        <v>192</v>
+      </c>
+      <c r="C310" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="D310" t="n">
         <v>0.008500000000000001</v>
       </c>
-      <c r="E309" t="n">
-        <v>0</v>
-      </c>
-      <c r="F309" t="n">
+      <c r="E310" t="n">
+        <v>0</v>
+      </c>
+      <c r="F310" t="n">
+        <v>61.64</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>S=c1sc2c([nH]1)cccc2</t>
+        </is>
+      </c>
+      <c r="B311" t="n">
+        <v>240</v>
+      </c>
+      <c r="C311" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="D311" t="n">
+        <v>0.0032</v>
+      </c>
+      <c r="E311" t="n">
+        <v>0</v>
+      </c>
+      <c r="F311" t="n">
+        <v>67.02</v>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>S=c1sc2c([nH]1)cccc2</t>
+        </is>
+      </c>
+      <c r="B312" t="n">
+        <v>240</v>
+      </c>
+      <c r="C312" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="D312" t="n">
+        <v>0.0042</v>
+      </c>
+      <c r="E312" t="n">
+        <v>0</v>
+      </c>
+      <c r="F312" t="n">
+        <v>51.13</v>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>S=c1sc2c([nH]1)cccc2</t>
+        </is>
+      </c>
+      <c r="B313" t="n">
+        <v>240</v>
+      </c>
+      <c r="C313" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="D313" t="n">
+        <v>0.0053</v>
+      </c>
+      <c r="E313" t="n">
+        <v>0</v>
+      </c>
+      <c r="F313" t="n">
+        <v>66.68000000000001</v>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>S=c1sc2c([nH]1)cccc2</t>
+        </is>
+      </c>
+      <c r="B314" t="n">
+        <v>240</v>
+      </c>
+      <c r="C314" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="D314" t="n">
+        <v>0.0065</v>
+      </c>
+      <c r="E314" t="n">
+        <v>0</v>
+      </c>
+      <c r="F314" t="n">
+        <v>67.58</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>S=c1sc2c([nH]1)cccc2</t>
+        </is>
+      </c>
+      <c r="B315" t="n">
+        <v>240</v>
+      </c>
+      <c r="C315" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="D315" t="n">
+        <v>0.0075</v>
+      </c>
+      <c r="E315" t="n">
+        <v>0</v>
+      </c>
+      <c r="F315" t="n">
+        <v>66.34</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>S=c1sc2c([nH]1)cccc2</t>
+        </is>
+      </c>
+      <c r="B316" t="n">
+        <v>240</v>
+      </c>
+      <c r="C316" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="D316" t="n">
+        <v>0.008500000000000001</v>
+      </c>
+      <c r="E316" t="n">
+        <v>0</v>
+      </c>
+      <c r="F316" t="n">
+        <v>68.66</v>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>S=c1sc2c([nH]1)cccc2</t>
+        </is>
+      </c>
+      <c r="B317" t="n">
+        <v>288</v>
+      </c>
+      <c r="C317" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="D317" t="n">
+        <v>0.0032</v>
+      </c>
+      <c r="E317" t="n">
+        <v>0</v>
+      </c>
+      <c r="F317" t="n">
+        <v>73.98999999999999</v>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>S=c1sc2c([nH]1)cccc2</t>
+        </is>
+      </c>
+      <c r="B318" t="n">
+        <v>288</v>
+      </c>
+      <c r="C318" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="D318" t="n">
+        <v>0.0042</v>
+      </c>
+      <c r="E318" t="n">
+        <v>0</v>
+      </c>
+      <c r="F318" t="n">
+        <v>62.52</v>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>S=c1sc2c([nH]1)cccc2</t>
+        </is>
+      </c>
+      <c r="B319" t="n">
+        <v>288</v>
+      </c>
+      <c r="C319" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="D319" t="n">
+        <v>0.0053</v>
+      </c>
+      <c r="E319" t="n">
+        <v>0</v>
+      </c>
+      <c r="F319" t="n">
+        <v>73.56</v>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>S=c1sc2c([nH]1)cccc2</t>
+        </is>
+      </c>
+      <c r="B320" t="n">
+        <v>288</v>
+      </c>
+      <c r="C320" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="D320" t="n">
+        <v>0.0065</v>
+      </c>
+      <c r="E320" t="n">
+        <v>0</v>
+      </c>
+      <c r="F320" t="n">
+        <v>72.56</v>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>S=c1sc2c([nH]1)cccc2</t>
+        </is>
+      </c>
+      <c r="B321" t="n">
+        <v>288</v>
+      </c>
+      <c r="C321" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="D321" t="n">
+        <v>0.0075</v>
+      </c>
+      <c r="E321" t="n">
+        <v>0</v>
+      </c>
+      <c r="F321" t="n">
+        <v>71.72</v>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>S=c1sc2c([nH]1)cccc2</t>
+        </is>
+      </c>
+      <c r="B322" t="n">
+        <v>288</v>
+      </c>
+      <c r="C322" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="D322" t="n">
+        <v>0.008500000000000001</v>
+      </c>
+      <c r="E322" t="n">
+        <v>0</v>
+      </c>
+      <c r="F322" t="n">
+        <v>73.38</v>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>S=c1sc2c([nH]1)cccc2</t>
+        </is>
+      </c>
+      <c r="B323" t="n">
+        <v>336</v>
+      </c>
+      <c r="C323" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="D323" t="n">
+        <v>0.0032</v>
+      </c>
+      <c r="E323" t="n">
+        <v>0</v>
+      </c>
+      <c r="F323" t="n">
+        <v>76.83</v>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>S=c1sc2c([nH]1)cccc2</t>
+        </is>
+      </c>
+      <c r="B324" t="n">
+        <v>336</v>
+      </c>
+      <c r="C324" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="D324" t="n">
+        <v>0.0042</v>
+      </c>
+      <c r="E324" t="n">
+        <v>0</v>
+      </c>
+      <c r="F324" t="n">
+        <v>69.75</v>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>S=c1sc2c([nH]1)cccc2</t>
+        </is>
+      </c>
+      <c r="B325" t="n">
+        <v>336</v>
+      </c>
+      <c r="C325" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="D325" t="n">
+        <v>0.0053</v>
+      </c>
+      <c r="E325" t="n">
+        <v>0</v>
+      </c>
+      <c r="F325" t="n">
+        <v>78.36</v>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>S=c1sc2c([nH]1)cccc2</t>
+        </is>
+      </c>
+      <c r="B326" t="n">
+        <v>336</v>
+      </c>
+      <c r="C326" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="D326" t="n">
+        <v>0.0065</v>
+      </c>
+      <c r="E326" t="n">
+        <v>0</v>
+      </c>
+      <c r="F326" t="n">
+        <v>75.54000000000001</v>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>S=c1sc2c([nH]1)cccc2</t>
+        </is>
+      </c>
+      <c r="B327" t="n">
+        <v>336</v>
+      </c>
+      <c r="C327" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="D327" t="n">
+        <v>0.0075</v>
+      </c>
+      <c r="E327" t="n">
+        <v>0</v>
+      </c>
+      <c r="F327" t="n">
+        <v>74.90000000000001</v>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>S=c1sc2c([nH]1)cccc2</t>
+        </is>
+      </c>
+      <c r="B328" t="n">
+        <v>336</v>
+      </c>
+      <c r="C328" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="D328" t="n">
+        <v>0.008500000000000001</v>
+      </c>
+      <c r="E328" t="n">
+        <v>0</v>
+      </c>
+      <c r="F328" t="n">
+        <v>76.88</v>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>S=c1sc2c([nH]1)cccc2</t>
+        </is>
+      </c>
+      <c r="B329" t="n">
+        <v>384</v>
+      </c>
+      <c r="C329" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="D329" t="n">
+        <v>0.0032</v>
+      </c>
+      <c r="E329" t="n">
+        <v>0</v>
+      </c>
+      <c r="F329" t="n">
+        <v>77.29000000000001</v>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>S=c1sc2c([nH]1)cccc2</t>
+        </is>
+      </c>
+      <c r="B330" t="n">
+        <v>384</v>
+      </c>
+      <c r="C330" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="D330" t="n">
+        <v>0.0042</v>
+      </c>
+      <c r="E330" t="n">
+        <v>0</v>
+      </c>
+      <c r="F330" t="n">
+        <v>70.59999999999999</v>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>S=c1sc2c([nH]1)cccc2</t>
+        </is>
+      </c>
+      <c r="B331" t="n">
+        <v>384</v>
+      </c>
+      <c r="C331" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="D331" t="n">
+        <v>0.0053</v>
+      </c>
+      <c r="E331" t="n">
+        <v>0</v>
+      </c>
+      <c r="F331" t="n">
+        <v>79.77</v>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>S=c1sc2c([nH]1)cccc2</t>
+        </is>
+      </c>
+      <c r="B332" t="n">
+        <v>384</v>
+      </c>
+      <c r="C332" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="D332" t="n">
+        <v>0.0065</v>
+      </c>
+      <c r="E332" t="n">
+        <v>0</v>
+      </c>
+      <c r="F332" t="n">
+        <v>76.72</v>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>S=c1sc2c([nH]1)cccc2</t>
+        </is>
+      </c>
+      <c r="B333" t="n">
+        <v>384</v>
+      </c>
+      <c r="C333" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="D333" t="n">
+        <v>0.0075</v>
+      </c>
+      <c r="E333" t="n">
+        <v>0</v>
+      </c>
+      <c r="F333" t="n">
+        <v>75.44</v>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>S=c1sc2c([nH]1)cccc2</t>
+        </is>
+      </c>
+      <c r="B334" t="n">
+        <v>384</v>
+      </c>
+      <c r="C334" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="D334" t="n">
+        <v>0.008500000000000001</v>
+      </c>
+      <c r="E334" t="n">
+        <v>0</v>
+      </c>
+      <c r="F334" t="n">
         <v>77.22</v>
       </c>
     </row>

</xml_diff>